<commit_message>
Add first few tests files
</commit_message>
<xml_diff>
--- a/docs/Test_Cases.xlsx
+++ b/docs/Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BIRVA\Documents\Birva\Upskill\Automation Testing\Banking_Automation_Repo\banking-test-automation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2443DFD-F53C-4062-A1D6-43C2225C2794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF581F9-7EAB-4B25-98A6-02978DCBDB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>TC ID</t>
   </si>
@@ -189,9 +189,6 @@
     <t>User is logged in successfully. "Accounts Overview" page is displayed</t>
   </si>
   <si>
-    <t>User is on login pageError message displayed: "The username and password could not be verified"Username: invalid123&lt;br&gt;Password: demo</t>
-  </si>
-  <si>
     <t>1. Enter invalid username&lt;br&gt;2. Enter any password&lt;br&gt;3. Click Login button</t>
   </si>
   <si>
@@ -229,6 +226,78 @@
   </si>
   <si>
     <t>Transfer successful message. Balance updated in both accounts</t>
+  </si>
+  <si>
+    <t>User is logged in with 2+ accounts</t>
+  </si>
+  <si>
+    <t>P2 - High</t>
+  </si>
+  <si>
+    <t>User is logged in with transactions</t>
+  </si>
+  <si>
+    <t>P3 - Medium</t>
+  </si>
+  <si>
+    <t>1. Enter valid username&lt;br&gt;2. Enter invalid password&lt;br&gt;3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Leave username blank&lt;br&gt;2. Leave password blank&lt;br&gt;3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Navigate to Accounts Overview&lt;br&gt;2. Observe account list</t>
+  </si>
+  <si>
+    <t>1. Click "Transfer Funds"&lt;br&gt;2. Enter amount&lt;br&gt;3. Select from account&lt;br&gt;4. Select to account&lt;br&gt;5. Click Transfer</t>
+  </si>
+  <si>
+    <t>1. Click "Transfer Funds"&lt;br&gt;2. Enter amount greater than balance&lt;br&gt;3. Select accounts&lt;br&gt;4. Click Transfer</t>
+  </si>
+  <si>
+    <t>1. Click "Transfer Funds"&lt;br&gt;2. Enter amount as 0&lt;br&gt;3. Select accounts&lt;br&gt;4. Click Transfer</t>
+  </si>
+  <si>
+    <t>1. Click "Accounts Overview"&lt;br&gt;2. Click any account number&lt;br&gt;3. View transaction details</t>
+  </si>
+  <si>
+    <t>1. Click "Open New Account"&lt;br&gt;2. Select account type&lt;br&gt;3. Select source account&lt;br&gt;4. Click "Open New Account"</t>
+  </si>
+  <si>
+    <t>1. Click "Update Contact Info"&lt;br&gt;2. Update phone number&lt;br&gt;3. Click "Update Profile"</t>
+  </si>
+  <si>
+    <t>1. Click "Request Loan"&lt;br&gt;2. Enter loan amount&lt;br&gt;3. Enter down payment&lt;br&gt;4. Click "Apply Now"</t>
+  </si>
+  <si>
+    <t>1. Click "Bill Pay"&lt;br&gt;2. Enter payee details&lt;br&gt;3. Enter amount&lt;br&gt;4. Select account&lt;br&gt;5. Click "Send Payment"</t>
+  </si>
+  <si>
+    <t>1. Click "Find Transactions"&lt;br&gt;2. Select account&lt;br&gt;3. Enter amount&lt;br&gt;4. Click "Find Transactions"</t>
+  </si>
+  <si>
+    <t>Error message: "Insufficient funds"</t>
+  </si>
+  <si>
+    <t>Error message or validation preventing transfer</t>
+  </si>
+  <si>
+    <t>Transaction history displayed with dates, descriptions, amounts</t>
+  </si>
+  <si>
+    <t>New account created successfully with account number displayed</t>
+  </si>
+  <si>
+    <t>Success message. Profile updated with new phone number</t>
+  </si>
+  <si>
+    <t>Loan request processed. Approval/denial status shown</t>
+  </si>
+  <si>
+    <t>Payment successful message. Balance deducted from account</t>
+  </si>
+  <si>
+    <t>Transactions matching the amount are displayed</t>
   </si>
 </sst>
 </file>
@@ -572,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +650,8 @@
     <col min="2" max="2" width="44.90625" customWidth="1"/>
     <col min="3" max="4" width="13.7265625" customWidth="1"/>
     <col min="5" max="5" width="33.90625" customWidth="1"/>
-    <col min="6" max="8" width="26.1796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29.08984375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="26.1796875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -650,16 +720,16 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -675,11 +745,17 @@
       <c r="D4" t="s">
         <v>41</v>
       </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -692,14 +768,20 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -712,14 +794,20 @@
       <c r="D6" t="s">
         <v>41</v>
       </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -732,14 +820,20 @@
       <c r="D7" t="s">
         <v>41</v>
       </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -752,12 +846,20 @@
       <c r="D8" t="s">
         <v>41</v>
       </c>
-      <c r="G8"/>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
+        <v>83</v>
+      </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -767,11 +869,23 @@
       <c r="C9" t="s">
         <v>39</v>
       </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" t="s">
+        <v>84</v>
+      </c>
       <c r="H9" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -781,11 +895,23 @@
       <c r="C10" t="s">
         <v>40</v>
       </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -796,10 +922,19 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -828,7 +963,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -838,11 +973,23 @@
       <c r="C13" t="s">
         <v>46</v>
       </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
       <c r="H13" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -852,11 +999,23 @@
       <c r="C14" t="s">
         <v>47</v>
       </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
       <c r="H14" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -866,11 +1025,23 @@
       <c r="C15" t="s">
         <v>48</v>
       </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
       <c r="H15" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -880,8 +1051,20 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>90</v>
+      </c>
       <c r="H16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>